<commit_message>
fixed import file excel
</commit_message>
<xml_diff>
--- a/UntukTesting Kab-Kota.xlsx
+++ b/UntukTesting Kab-Kota.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\keprakdibi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\keprakdibi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -916,368 +916,371 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="E1" s="70" t="s">
         <v>69</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
+      <c r="B2" s="2">
+        <v>276</v>
+      </c>
       <c r="C2" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D2" s="2">
-        <v>277</v>
-      </c>
-      <c r="E2" s="2">
         <v>278</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
+        <v>279</v>
+      </c>
       <c r="G2" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H2" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="I2" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="J2" s="2">
-        <v>282</v>
-      </c>
-      <c r="K2" s="2">
         <v>283</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
+      <c r="B3" s="3">
+        <v>1425462.9285254199</v>
+      </c>
       <c r="C3" s="3">
-        <v>1425462.9285254199</v>
+        <v>475578.52681089001</v>
       </c>
       <c r="D3" s="3">
-        <v>475578.52681089001</v>
-      </c>
-      <c r="E3" s="3">
         <v>852341.27035604999</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
+        <v>488984.31556771003</v>
+      </c>
       <c r="G3" s="3">
-        <v>488984.31556771003</v>
+        <v>673678.12760280003</v>
       </c>
       <c r="H3" s="3">
-        <v>673678.12760280003</v>
+        <v>447067.23284831998</v>
       </c>
       <c r="I3" s="3">
-        <v>447067.23284831998</v>
+        <v>784878.35384201002</v>
       </c>
       <c r="J3" s="3">
-        <v>784878.35384201002</v>
-      </c>
-      <c r="K3" s="3">
         <v>903747.42379760998</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="B4" s="3">
+        <v>979194.61082824995</v>
+      </c>
       <c r="C4" s="3">
-        <v>979194.61082824995</v>
+        <v>16252.951099100001</v>
       </c>
       <c r="D4" s="3">
-        <v>16252.951099100001</v>
-      </c>
-      <c r="E4" s="3">
         <v>86962.00169515</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
+        <v>34380.822968319997</v>
+      </c>
       <c r="G4" s="3">
-        <v>34380.822968319997</v>
+        <v>62696.40942692</v>
       </c>
       <c r="H4" s="3">
-        <v>62696.40942692</v>
+        <v>31331.31942634</v>
       </c>
       <c r="I4" s="3">
-        <v>31331.31942634</v>
+        <v>116860.67833651</v>
       </c>
       <c r="J4" s="3">
-        <v>116860.67833651</v>
-      </c>
-      <c r="K4" s="3">
         <v>260482.61620185</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>12</v>
       </c>
+      <c r="B5" s="3">
+        <v>877403.36755612004</v>
+      </c>
       <c r="C5" s="3">
-        <v>877403.36755612004</v>
+        <v>2978.3116126999998</v>
       </c>
       <c r="D5" s="3">
-        <v>2978.3116126999998</v>
-      </c>
-      <c r="E5" s="3">
         <v>19837.345699419999</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <v>5294.4072619999997</v>
+      </c>
       <c r="G5" s="3">
-        <v>5294.4072619999997</v>
+        <v>33221.964175499998</v>
       </c>
       <c r="H5" s="3">
-        <v>33221.964175499998</v>
+        <v>3683.645696</v>
       </c>
       <c r="I5" s="3">
-        <v>3683.645696</v>
+        <v>23703.37543</v>
       </c>
       <c r="J5" s="3">
-        <v>23703.37543</v>
-      </c>
-      <c r="K5" s="3">
         <v>169581.41471617002</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
+      <c r="B6" s="3">
+        <v>42421.693220000001</v>
+      </c>
       <c r="C6" s="3">
-        <v>42421.693220000001</v>
+        <v>7738.5640418699995</v>
       </c>
       <c r="D6" s="3">
-        <v>7738.5640418699995</v>
-      </c>
-      <c r="E6" s="3">
         <v>10370.220475</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>8129.8038672900002</v>
+      </c>
       <c r="G6" s="3">
-        <v>8129.8038672900002</v>
+        <v>8203.4463799599998</v>
       </c>
       <c r="H6" s="3">
-        <v>8203.4463799599998</v>
+        <v>20122.661041619998</v>
       </c>
       <c r="I6" s="3">
-        <v>20122.661041619998</v>
+        <v>16536.413339040002</v>
       </c>
       <c r="J6" s="3">
-        <v>16536.413339040002</v>
-      </c>
-      <c r="K6" s="3">
         <v>26191.507818999999</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>14</v>
       </c>
+      <c r="B7" s="3">
+        <v>29815.039606509999</v>
+      </c>
       <c r="C7" s="3">
-        <v>29815.039606509999</v>
+        <v>1947.55553725</v>
       </c>
       <c r="D7" s="3">
-        <v>1947.55553725</v>
-      </c>
-      <c r="E7" s="3">
         <v>6657.57955597</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <v>2305.40923969</v>
+      </c>
       <c r="G7" s="3">
-        <v>2305.40923969</v>
+        <v>7460.3863507899996</v>
       </c>
       <c r="H7" s="3">
-        <v>7460.3863507899996</v>
+        <v>4166.11884775</v>
       </c>
       <c r="I7" s="3">
-        <v>4166.11884775</v>
+        <v>4788.0261594499998</v>
       </c>
       <c r="J7" s="3">
-        <v>4788.0261594499998</v>
-      </c>
-      <c r="K7" s="3">
         <v>7831.4452366599999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>15</v>
       </c>
+      <c r="B8" s="3">
+        <v>29554.510445619999</v>
+      </c>
       <c r="C8" s="3">
-        <v>29554.510445619999</v>
+        <v>3588.5199072800001</v>
       </c>
       <c r="D8" s="3">
-        <v>3588.5199072800001</v>
-      </c>
-      <c r="E8" s="3">
         <v>50096.855964760005</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>18651.202599339998</v>
+      </c>
       <c r="G8" s="3">
-        <v>18651.202599339998</v>
+        <v>13810.61252067</v>
       </c>
       <c r="H8" s="3">
-        <v>13810.61252067</v>
+        <v>3358.8938409699999</v>
       </c>
       <c r="I8" s="3">
-        <v>3358.8938409699999</v>
+        <v>71832.863408019999</v>
       </c>
       <c r="J8" s="3">
-        <v>71832.863408019999</v>
-      </c>
-      <c r="K8" s="3">
         <v>56878.248430019994</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
+      <c r="B9" s="3">
+        <v>413254.93873716996</v>
+      </c>
       <c r="C9" s="3">
-        <v>413254.93873716996</v>
+        <v>459325.57571179001</v>
       </c>
       <c r="D9" s="3">
-        <v>459325.57571179001</v>
-      </c>
-      <c r="E9" s="3">
         <v>764526.7441289</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>452893.45259939</v>
+      </c>
       <c r="G9" s="3">
-        <v>452893.45259939</v>
+        <v>607036.06418588001</v>
       </c>
       <c r="H9" s="3">
-        <v>607036.06418588001</v>
+        <v>414181.85342197999</v>
       </c>
       <c r="I9" s="3">
-        <v>414181.85342197999</v>
+        <v>663197.85550549999</v>
       </c>
       <c r="J9" s="3">
-        <v>663197.85550549999</v>
-      </c>
-      <c r="K9" s="3">
         <v>641104.25359575998</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="B10" s="3">
+        <v>322095.76246599999</v>
+      </c>
       <c r="C10" s="3">
-        <v>322095.76246599999</v>
+        <v>345929.60843099997</v>
       </c>
       <c r="D10" s="3">
-        <v>345929.60843099997</v>
-      </c>
-      <c r="E10" s="3">
         <v>623176.27684900002</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
+        <v>371898.146572</v>
+      </c>
       <c r="G10" s="3">
-        <v>371898.146572</v>
+        <v>460411.445611</v>
       </c>
       <c r="H10" s="3">
-        <v>460411.445611</v>
+        <v>334470.47901200003</v>
       </c>
       <c r="I10" s="3">
-        <v>334470.47901200003</v>
+        <v>513683.61212499999</v>
       </c>
       <c r="J10" s="3">
-        <v>513683.61212499999</v>
-      </c>
-      <c r="K10" s="3">
         <v>499195.16681999998</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="B11" s="3">
+        <v>186131.73567200001</v>
+      </c>
       <c r="C11" s="3">
-        <v>186131.73567200001</v>
+        <v>23348.293977000001</v>
       </c>
       <c r="D11" s="3">
-        <v>23348.293977000001</v>
-      </c>
-      <c r="E11" s="3">
         <v>44526.528337999996</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <v>28476.980060999998</v>
+      </c>
       <c r="G11" s="3">
-        <v>28476.980060999998</v>
+        <v>29406.247100000001</v>
       </c>
       <c r="H11" s="3">
-        <v>29406.247100000001</v>
+        <v>18880.825218000002</v>
       </c>
       <c r="I11" s="3">
-        <v>18880.825218000002</v>
+        <v>35693.101330999998</v>
       </c>
       <c r="J11" s="3">
-        <v>35693.101330999998</v>
-      </c>
-      <c r="K11" s="3">
         <v>148205.65602600001</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="B12" s="3">
+        <v>428.35879399999999</v>
+      </c>
       <c r="C12" s="3">
-        <v>428.35879399999999</v>
+        <v>448.538454</v>
       </c>
       <c r="D12" s="3">
-        <v>448.538454</v>
-      </c>
-      <c r="E12" s="3">
         <v>133.33451099999999</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
+        <v>133.33451099999999</v>
+      </c>
       <c r="G12" s="3">
         <v>133.33451099999999</v>
       </c>
       <c r="H12" s="3">
-        <v>133.33451099999999</v>
+        <v>428.35879399999999</v>
       </c>
       <c r="I12" s="3">
         <v>428.35879399999999</v>
@@ -1285,114 +1288,114 @@
       <c r="J12" s="3">
         <v>428.35879399999999</v>
       </c>
-      <c r="K12" s="3">
-        <v>428.35879399999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>20</v>
       </c>
+      <c r="B13" s="3">
+        <v>131919.568</v>
+      </c>
       <c r="C13" s="3">
-        <v>131919.568</v>
+        <v>292695.47600000002</v>
       </c>
       <c r="D13" s="3">
-        <v>292695.47600000002</v>
-      </c>
-      <c r="E13" s="3">
         <v>512748.21399999998</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>308567.03200000001</v>
+      </c>
       <c r="G13" s="3">
-        <v>308567.03200000001</v>
+        <v>374537.06400000001</v>
       </c>
       <c r="H13" s="3">
-        <v>374537.06400000001</v>
+        <v>285662.09499999997</v>
       </c>
       <c r="I13" s="3">
-        <v>285662.09499999997</v>
+        <v>429919.45199999999</v>
       </c>
       <c r="J13" s="3">
-        <v>429919.45199999999</v>
-      </c>
-      <c r="K13" s="3">
         <v>336125.55200000003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>21</v>
       </c>
+      <c r="B14" s="3">
+        <v>3616.1</v>
+      </c>
       <c r="C14" s="3">
-        <v>3616.1</v>
+        <v>29437.3</v>
       </c>
       <c r="D14" s="3">
-        <v>29437.3</v>
-      </c>
-      <c r="E14" s="3">
         <v>65768.2</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
+        <v>34720.800000000003</v>
+      </c>
       <c r="G14" s="3">
-        <v>34720.800000000003</v>
+        <v>56334.8</v>
       </c>
       <c r="H14" s="3">
-        <v>56334.8</v>
+        <v>29499.200000000001</v>
       </c>
       <c r="I14" s="3">
-        <v>29499.200000000001</v>
+        <v>47642.7</v>
       </c>
       <c r="J14" s="3">
-        <v>47642.7</v>
-      </c>
-      <c r="K14" s="3">
         <v>14435.6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>22</v>
       </c>
+      <c r="B15" s="3">
+        <v>45975.460518</v>
+      </c>
       <c r="C15" s="3">
-        <v>45975.460518</v>
+        <v>68532.909893999997</v>
       </c>
       <c r="D15" s="3">
-        <v>68532.909893999997</v>
-      </c>
-      <c r="E15" s="3">
         <v>72218.756399999998</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
+        <v>28413.200400000002</v>
+      </c>
       <c r="G15" s="3">
-        <v>28413.200400000002</v>
+        <v>81921.528693</v>
       </c>
       <c r="H15" s="3">
-        <v>81921.528693</v>
+        <v>36410.124799999998</v>
       </c>
       <c r="I15" s="3">
-        <v>36410.124799999998</v>
+        <v>88718.123238</v>
       </c>
       <c r="J15" s="3">
-        <v>88718.123238</v>
-      </c>
-      <c r="K15" s="3">
         <v>78385.282600000006</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
       <c r="C16" s="3">
         <v>0</v>
       </c>
       <c r="D16" s="3">
         <v>0</v>
       </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
       <c r="G16" s="3">
         <v>0</v>
       </c>
@@ -1405,114 +1408,114 @@
       <c r="J16" s="3">
         <v>0</v>
       </c>
-      <c r="K16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="B17" s="3">
+        <v>45975.460518</v>
+      </c>
       <c r="C17" s="3">
-        <v>45975.460518</v>
+        <v>68532.909893999997</v>
       </c>
       <c r="D17" s="3">
-        <v>68532.909893999997</v>
-      </c>
-      <c r="E17" s="3">
         <v>72218.756399999998</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3">
+        <v>28413.200400000002</v>
+      </c>
       <c r="G17" s="3">
-        <v>28413.200400000002</v>
+        <v>81921.528693</v>
       </c>
       <c r="H17" s="3">
-        <v>81921.528693</v>
+        <v>36410.124799999998</v>
       </c>
       <c r="I17" s="3">
-        <v>36410.124799999998</v>
+        <v>88718.123238</v>
       </c>
       <c r="J17" s="3">
-        <v>88718.123238</v>
-      </c>
-      <c r="K17" s="3">
         <v>78385.282600000006</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>25</v>
       </c>
+      <c r="B18" s="3">
+        <v>45183.71575317</v>
+      </c>
       <c r="C18" s="3">
-        <v>45183.71575317</v>
+        <v>44863.057386790002</v>
       </c>
       <c r="D18" s="3">
-        <v>44863.057386790002</v>
-      </c>
-      <c r="E18" s="3">
         <v>69131.710879899998</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3">
+        <v>52582.105627389996</v>
+      </c>
       <c r="G18" s="3">
-        <v>52582.105627389996</v>
+        <v>64703.089881879998</v>
       </c>
       <c r="H18" s="3">
-        <v>64703.089881879998</v>
+        <v>43301.249609980005</v>
       </c>
       <c r="I18" s="3">
-        <v>43301.249609980005</v>
+        <v>60796.120142500004</v>
       </c>
       <c r="J18" s="3">
-        <v>60796.120142500004</v>
-      </c>
-      <c r="K18" s="3">
         <v>63523.80417576</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>26</v>
       </c>
+      <c r="B19" s="3">
+        <v>45183.71575317</v>
+      </c>
       <c r="C19" s="3">
-        <v>45183.71575317</v>
+        <v>43104.517386790001</v>
       </c>
       <c r="D19" s="3">
-        <v>43104.517386790001</v>
-      </c>
-      <c r="E19" s="3">
         <v>63989.730879900002</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3">
+        <v>52582.105627389996</v>
+      </c>
       <c r="G19" s="3">
-        <v>52582.105627389996</v>
+        <v>64703.089881879998</v>
       </c>
       <c r="H19" s="3">
-        <v>64703.089881879998</v>
+        <v>43301.249609980005</v>
       </c>
       <c r="I19" s="3">
-        <v>43301.249609980005</v>
+        <v>60796.120142500004</v>
       </c>
       <c r="J19" s="3">
-        <v>60796.120142500004</v>
-      </c>
-      <c r="K19" s="3">
         <v>63523.80417576</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>1758.54</v>
       </c>
       <c r="D20" s="3">
-        <v>1758.54</v>
-      </c>
-      <c r="E20" s="3">
         <v>5141.9799999999996</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
       <c r="G20" s="3">
         <v>0</v>
       </c>
@@ -1525,84 +1528,84 @@
       <c r="J20" s="3">
         <v>0</v>
       </c>
-      <c r="K20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>28</v>
       </c>
+      <c r="B21" s="3">
+        <v>33013.378960000002</v>
+      </c>
       <c r="C21" s="3">
-        <v>33013.378960000002</v>
+        <v>0</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
         <v>852.52453200000002</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <v>1710.04</v>
+      </c>
       <c r="G21" s="3">
-        <v>1710.04</v>
+        <v>3945.6539899999998</v>
       </c>
       <c r="H21" s="3">
-        <v>3945.6539899999998</v>
+        <v>1554.06</v>
       </c>
       <c r="I21" s="3">
-        <v>1554.06</v>
+        <v>4819.82</v>
       </c>
       <c r="J21" s="3">
-        <v>4819.82</v>
-      </c>
-      <c r="K21" s="3">
         <v>2160.5540000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>29</v>
       </c>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
       <c r="C22" s="3">
         <v>0</v>
       </c>
       <c r="D22" s="3">
         <v>0</v>
       </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
       <c r="G22" s="3">
-        <v>0</v>
+        <v>1134.95399</v>
       </c>
       <c r="H22" s="3">
-        <v>1134.95399</v>
+        <v>0</v>
       </c>
       <c r="I22" s="3">
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <v>0</v>
-      </c>
-      <c r="K22" s="3">
         <v>937.85400000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>30</v>
       </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
       <c r="C23" s="3">
         <v>0</v>
       </c>
       <c r="D23" s="3">
         <v>0</v>
       </c>
-      <c r="E23" s="3">
-        <v>0</v>
-      </c>
-      <c r="F23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
       <c r="G23" s="3">
         <v>0</v>
       </c>
@@ -1615,206 +1618,206 @@
       <c r="J23" s="3">
         <v>0</v>
       </c>
-      <c r="K23" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>31</v>
       </c>
+      <c r="B24" s="3">
+        <v>33013.378960000002</v>
+      </c>
       <c r="C24" s="3">
-        <v>33013.378960000002</v>
+        <v>0</v>
       </c>
       <c r="D24" s="3">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3">
         <v>852.52453200000002</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3">
+        <v>1710.04</v>
+      </c>
       <c r="G24" s="3">
-        <v>1710.04</v>
+        <v>2810.7</v>
       </c>
       <c r="H24" s="3">
-        <v>2810.7</v>
+        <v>1554.06</v>
       </c>
       <c r="I24" s="3">
-        <v>1554.06</v>
+        <v>4819.82</v>
       </c>
       <c r="J24" s="3">
-        <v>4819.82</v>
-      </c>
-      <c r="K24" s="3">
         <v>1222.7</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>32</v>
       </c>
+      <c r="B25" s="3">
+        <v>1202670.8394279899</v>
+      </c>
       <c r="C25" s="3">
-        <v>1202670.8394279899</v>
+        <v>445083.985239</v>
       </c>
       <c r="D25" s="3">
-        <v>445083.985239</v>
-      </c>
-      <c r="E25" s="3">
         <v>834791.00169143011</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3">
+        <v>478614.32016500999</v>
+      </c>
       <c r="G25" s="3">
-        <v>478614.32016500999</v>
+        <v>630249.35694481002</v>
       </c>
       <c r="H25" s="3">
-        <v>630249.35694481002</v>
+        <v>441661.03913599998</v>
       </c>
       <c r="I25" s="3">
-        <v>441661.03913599998</v>
+        <v>771801.07219154004</v>
       </c>
       <c r="J25" s="3">
-        <v>771801.07219154004</v>
-      </c>
-      <c r="K25" s="3">
         <v>927540.2522240699</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>33</v>
       </c>
+      <c r="B26" s="3">
+        <v>1023940.69387899</v>
+      </c>
       <c r="C26" s="3">
-        <v>1023940.69387899</v>
+        <v>375478.02351000003</v>
       </c>
       <c r="D26" s="3">
-        <v>375478.02351000003</v>
-      </c>
-      <c r="E26" s="3">
         <v>787159.24641343008</v>
       </c>
-      <c r="F26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <v>419986.43604256999</v>
+      </c>
       <c r="G26" s="3">
-        <v>419986.43604256999</v>
+        <v>551026.81322181004</v>
       </c>
       <c r="H26" s="3">
-        <v>551026.81322181004</v>
+        <v>398624.74049</v>
       </c>
       <c r="I26" s="3">
-        <v>398624.74049</v>
+        <v>696284.97340054007</v>
       </c>
       <c r="J26" s="3">
-        <v>696284.97340054007</v>
-      </c>
-      <c r="K26" s="3">
         <v>861039.50428507</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>34</v>
       </c>
+      <c r="B27" s="3">
+        <v>602436.47726493992</v>
+      </c>
       <c r="C27" s="3">
-        <v>602436.47726493992</v>
+        <v>290349.11604300002</v>
       </c>
       <c r="D27" s="3">
-        <v>290349.11604300002</v>
-      </c>
-      <c r="E27" s="3">
         <v>602221.89502519998</v>
       </c>
-      <c r="F27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3">
+        <v>284113.03134789004</v>
+      </c>
       <c r="G27" s="3">
-        <v>284113.03134789004</v>
+        <v>439685.20911699999</v>
       </c>
       <c r="H27" s="3">
-        <v>439685.20911699999</v>
+        <v>291087.67660499999</v>
       </c>
       <c r="I27" s="3">
-        <v>291087.67660499999</v>
+        <v>516415.65846031002</v>
       </c>
       <c r="J27" s="3">
-        <v>516415.65846031002</v>
-      </c>
-      <c r="K27" s="3">
         <v>534173.58107398998</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>35</v>
       </c>
+      <c r="B28" s="3">
+        <v>203008.44517600001</v>
+      </c>
       <c r="C28" s="3">
-        <v>203008.44517600001</v>
+        <v>52053.621735000001</v>
       </c>
       <c r="D28" s="3">
-        <v>52053.621735000001</v>
-      </c>
-      <c r="E28" s="3">
         <v>129954.65547445</v>
       </c>
-      <c r="F28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3">
+        <v>86616.291392309999</v>
+      </c>
       <c r="G28" s="3">
-        <v>86616.291392309999</v>
+        <v>69085.306398000001</v>
       </c>
       <c r="H28" s="3">
-        <v>69085.306398000001</v>
+        <v>68198.774124999996</v>
       </c>
       <c r="I28" s="3">
-        <v>68198.774124999996</v>
+        <v>101150.93320347001</v>
       </c>
       <c r="J28" s="3">
-        <v>101150.93320347001</v>
-      </c>
-      <c r="K28" s="3">
         <v>240646.022015</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>36</v>
       </c>
+      <c r="B29" s="3">
+        <v>3621.6878470000001</v>
+      </c>
       <c r="C29" s="3">
-        <v>3621.6878470000001</v>
+        <v>0</v>
       </c>
       <c r="D29" s="3">
-        <v>0</v>
-      </c>
-      <c r="E29" s="3">
         <v>156.88591428000001</v>
       </c>
-      <c r="F29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
       <c r="G29" s="3">
-        <v>0</v>
+        <v>159.79855881</v>
       </c>
       <c r="H29" s="3">
-        <v>159.79855881</v>
+        <v>0</v>
       </c>
       <c r="I29" s="3">
-        <v>0</v>
+        <v>535.05716418999998</v>
       </c>
       <c r="J29" s="3">
-        <v>535.05716418999998</v>
-      </c>
-      <c r="K29" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>37</v>
       </c>
+      <c r="B30" s="3">
+        <v>754.88338999999996</v>
+      </c>
       <c r="C30" s="3">
-        <v>754.88338999999996</v>
+        <v>165</v>
       </c>
       <c r="D30" s="3">
-        <v>165</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0</v>
-      </c>
-      <c r="F30" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3">
+        <v>33.232500000000002</v>
+      </c>
       <c r="G30" s="3">
-        <v>33.232500000000002</v>
+        <v>0</v>
       </c>
       <c r="H30" s="3">
         <v>0</v>
@@ -1823,296 +1826,296 @@
         <v>0</v>
       </c>
       <c r="J30" s="3">
-        <v>0</v>
-      </c>
-      <c r="K30" s="3">
         <v>348</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>38</v>
       </c>
+      <c r="B31" s="3">
+        <v>35167.765332900002</v>
+      </c>
       <c r="C31" s="3">
-        <v>35167.765332900002</v>
+        <v>15064.012731999999</v>
       </c>
       <c r="D31" s="3">
-        <v>15064.012731999999</v>
-      </c>
-      <c r="E31" s="3">
         <v>9885.7000000000007</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3">
+        <v>30361.4025</v>
+      </c>
       <c r="G31" s="3">
-        <v>30361.4025</v>
+        <v>16932.356390000001</v>
       </c>
       <c r="H31" s="3">
-        <v>16932.356390000001</v>
+        <v>9649.2226300000002</v>
       </c>
       <c r="I31" s="3">
-        <v>9649.2226300000002</v>
+        <v>19358.113566</v>
       </c>
       <c r="J31" s="3">
-        <v>19358.113566</v>
-      </c>
-      <c r="K31" s="3">
         <v>24677.679671999998</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>39</v>
       </c>
+      <c r="B32" s="3">
+        <v>33852.354427959996</v>
+      </c>
       <c r="C32" s="3">
-        <v>33852.354427959996</v>
+        <v>17846.273000000001</v>
       </c>
       <c r="D32" s="3">
-        <v>17846.273000000001</v>
-      </c>
-      <c r="E32" s="3">
         <v>8518.7000000000007</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3">
+        <v>18862.47830237</v>
+      </c>
       <c r="G32" s="3">
-        <v>18862.47830237</v>
+        <v>16160.6</v>
       </c>
       <c r="H32" s="3">
-        <v>16160.6</v>
+        <v>13918.282233</v>
       </c>
       <c r="I32" s="3">
-        <v>13918.282233</v>
+        <v>8916.5</v>
       </c>
       <c r="J32" s="3">
-        <v>8916.5</v>
-      </c>
-      <c r="K32" s="3">
         <v>21955.507000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>40</v>
       </c>
+      <c r="B33" s="3">
+        <v>145099.08044019001</v>
+      </c>
       <c r="C33" s="3">
-        <v>145099.08044019001</v>
+        <v>0</v>
       </c>
       <c r="D33" s="3">
-        <v>0</v>
-      </c>
-      <c r="E33" s="3">
         <v>36421.4099995</v>
       </c>
-      <c r="F33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
       <c r="G33" s="3">
-        <v>0</v>
+        <v>9003.5427579999996</v>
       </c>
       <c r="H33" s="3">
-        <v>9003.5427579999996</v>
+        <v>15770.784897</v>
       </c>
       <c r="I33" s="3">
-        <v>15770.784897</v>
+        <v>49908.711006569996</v>
       </c>
       <c r="J33" s="3">
-        <v>49908.711006569996</v>
-      </c>
-      <c r="K33" s="3">
         <v>39238.714524080002</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>41</v>
       </c>
+      <c r="B34" s="4">
+        <v>176302.823279</v>
+      </c>
       <c r="C34" s="4">
-        <v>176302.823279</v>
+        <v>68608.586469000002</v>
       </c>
       <c r="D34" s="4">
-        <v>68608.586469000002</v>
-      </c>
-      <c r="E34" s="4">
         <v>47207.570277999999</v>
       </c>
-      <c r="F34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4">
+        <v>58163.280122440003</v>
+      </c>
       <c r="G34" s="4">
-        <v>58163.280122440003</v>
+        <v>77507.953901000001</v>
       </c>
       <c r="H34" s="4">
-        <v>77507.953901000001</v>
+        <v>42555.098645999999</v>
       </c>
       <c r="I34" s="4">
-        <v>42555.098645999999</v>
+        <v>74637.534171000007</v>
       </c>
       <c r="J34" s="4">
-        <v>74637.534171000007</v>
-      </c>
-      <c r="K34" s="4">
         <v>65756.361239000005</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>42</v>
       </c>
+      <c r="B35" s="3">
+        <v>8862.75</v>
+      </c>
       <c r="C35" s="3">
-        <v>8862.75</v>
+        <v>0</v>
       </c>
       <c r="D35" s="3">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3">
         <v>1581</v>
       </c>
-      <c r="F35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
       <c r="G35" s="3">
-        <v>0</v>
+        <v>1489.75</v>
       </c>
       <c r="H35" s="3">
-        <v>1489.75</v>
+        <v>231</v>
       </c>
       <c r="I35" s="3">
-        <v>231</v>
+        <v>2235.0430000000001</v>
       </c>
       <c r="J35" s="3">
-        <v>2235.0430000000001</v>
-      </c>
-      <c r="K35" s="3">
         <v>47.457644000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>43</v>
       </c>
+      <c r="B36" s="3">
+        <v>29084.06899</v>
+      </c>
       <c r="C36" s="3">
-        <v>29084.06899</v>
+        <v>8228.6364410000006</v>
       </c>
       <c r="D36" s="3">
-        <v>8228.6364410000006</v>
-      </c>
-      <c r="E36" s="3">
         <v>17796.005978000001</v>
       </c>
-      <c r="F36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3">
+        <v>7184.9948199999999</v>
+      </c>
       <c r="G36" s="3">
-        <v>7184.9948199999999</v>
+        <v>8196.3219700000009</v>
       </c>
       <c r="H36" s="3">
-        <v>8196.3219700000009</v>
+        <v>16878.906625</v>
       </c>
       <c r="I36" s="3">
-        <v>16878.906625</v>
+        <v>20392.204570999998</v>
       </c>
       <c r="J36" s="3">
-        <v>20392.204570999998</v>
-      </c>
-      <c r="K36" s="3">
         <v>32607.921735</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="B37" s="3">
+        <v>75905.876340999996</v>
+      </c>
       <c r="C37" s="3">
-        <v>75905.876340999996</v>
+        <v>4793.62</v>
       </c>
       <c r="D37" s="3">
-        <v>4793.62</v>
-      </c>
-      <c r="E37" s="3">
         <v>6907.8395</v>
       </c>
-      <c r="F37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3">
+        <v>20730.081302439998</v>
+      </c>
       <c r="G37" s="3">
-        <v>20730.081302439998</v>
+        <v>8844.8465309999992</v>
       </c>
       <c r="H37" s="3">
-        <v>8844.8465309999992</v>
+        <v>14605.251131999999</v>
       </c>
       <c r="I37" s="3">
-        <v>14605.251131999999</v>
+        <v>7939.0150000000003</v>
       </c>
       <c r="J37" s="3">
-        <v>7939.0150000000003</v>
-      </c>
-      <c r="K37" s="3">
         <v>18383.70019</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>45</v>
       </c>
+      <c r="B38" s="3">
+        <v>60618.426650000001</v>
+      </c>
       <c r="C38" s="3">
-        <v>60618.426650000001</v>
+        <v>55290.660027999998</v>
       </c>
       <c r="D38" s="3">
-        <v>55290.660027999998</v>
-      </c>
-      <c r="E38" s="3">
         <v>20341.100399999999</v>
       </c>
-      <c r="F38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3">
+        <v>30073.156999999999</v>
+      </c>
       <c r="G38" s="3">
-        <v>30073.156999999999</v>
+        <v>58449.669900000001</v>
       </c>
       <c r="H38" s="3">
-        <v>58449.669900000001</v>
+        <v>10814.709889</v>
       </c>
       <c r="I38" s="3">
-        <v>10814.709889</v>
+        <v>43945.882599999997</v>
       </c>
       <c r="J38" s="3">
-        <v>43945.882599999997</v>
-      </c>
-      <c r="K38" s="3">
         <v>11242.208769999999</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>46</v>
       </c>
+      <c r="B39" s="3">
+        <v>1831.701298</v>
+      </c>
       <c r="C39" s="3">
-        <v>1831.701298</v>
+        <v>295.67</v>
       </c>
       <c r="D39" s="3">
-        <v>295.67</v>
-      </c>
-      <c r="E39" s="3">
         <v>581.62440000000004</v>
       </c>
-      <c r="F39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3">
+        <v>175.047</v>
+      </c>
       <c r="G39" s="3">
-        <v>175.047</v>
+        <v>24.961500000000001</v>
       </c>
       <c r="H39" s="3">
-        <v>24.961500000000001</v>
+        <v>25.231000000000002</v>
       </c>
       <c r="I39" s="3">
-        <v>25.231000000000002</v>
+        <v>125.389</v>
       </c>
       <c r="J39" s="3">
-        <v>125.389</v>
-      </c>
-      <c r="K39" s="3">
         <v>3475.0729000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>47</v>
       </c>
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
       <c r="C40" s="3">
         <v>0</v>
       </c>
       <c r="D40" s="3">
         <v>0</v>
       </c>
-      <c r="E40" s="3">
-        <v>0</v>
-      </c>
-      <c r="F40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3">
+        <v>0</v>
+      </c>
       <c r="G40" s="3">
         <v>0</v>
       </c>
@@ -2125,29 +2128,29 @@
       <c r="J40" s="3">
         <v>0</v>
       </c>
-      <c r="K40" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
       <c r="C41" s="3">
         <v>0</v>
       </c>
       <c r="D41" s="3">
         <v>0</v>
       </c>
-      <c r="E41" s="3">
-        <v>0</v>
-      </c>
-      <c r="F41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3">
+        <v>0</v>
+      </c>
       <c r="G41" s="3">
-        <v>0</v>
+        <v>502.404</v>
       </c>
       <c r="H41" s="3">
-        <v>502.404</v>
+        <v>0</v>
       </c>
       <c r="I41" s="3">
         <v>0</v>
@@ -2155,179 +2158,179 @@
       <c r="J41" s="3">
         <v>0</v>
       </c>
-      <c r="K41" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>49</v>
       </c>
+      <c r="B42" s="3">
+        <v>2427.3222700000001</v>
+      </c>
       <c r="C42" s="3">
-        <v>2427.3222700000001</v>
+        <v>997.37526000000003</v>
       </c>
       <c r="D42" s="3">
-        <v>997.37526000000003</v>
-      </c>
-      <c r="E42" s="3">
         <v>424.185</v>
       </c>
-      <c r="F42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3">
+        <v>464.60399999999998</v>
+      </c>
       <c r="G42" s="3">
-        <v>464.60399999999998</v>
+        <v>1714.5898219999999</v>
       </c>
       <c r="H42" s="3">
-        <v>1714.5898219999999</v>
+        <v>481.2</v>
       </c>
       <c r="I42" s="3">
-        <v>481.2</v>
+        <v>878.56461999999999</v>
       </c>
       <c r="J42" s="3">
-        <v>878.56461999999999</v>
-      </c>
-      <c r="K42" s="3">
         <v>744.38670000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>49</v>
       </c>
+      <c r="B43" s="3">
+        <v>2427.3222700000001</v>
+      </c>
       <c r="C43" s="3">
-        <v>2427.3222700000001</v>
+        <v>997.37526000000003</v>
       </c>
       <c r="D43" s="3">
-        <v>997.37526000000003</v>
-      </c>
-      <c r="E43" s="3">
         <v>424.185</v>
       </c>
-      <c r="F43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3">
+        <v>464.60399999999998</v>
+      </c>
       <c r="G43" s="3">
-        <v>464.60399999999998</v>
+        <v>1714.5898219999999</v>
       </c>
       <c r="H43" s="3">
-        <v>1714.5898219999999</v>
+        <v>481.2</v>
       </c>
       <c r="I43" s="3">
-        <v>481.2</v>
+        <v>878.56461999999999</v>
       </c>
       <c r="J43" s="3">
-        <v>878.56461999999999</v>
-      </c>
-      <c r="K43" s="3">
         <v>744.38670000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>50</v>
       </c>
+      <c r="B44" s="3">
+        <v>116387.51151544</v>
+      </c>
       <c r="C44" s="3">
-        <v>116387.51151544</v>
+        <v>25615.927377960001</v>
       </c>
       <c r="D44" s="3">
-        <v>25615.927377960001</v>
-      </c>
-      <c r="E44" s="3">
         <v>2749.9935245799998</v>
       </c>
-      <c r="F44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3">
+        <v>17693.456552400003</v>
+      </c>
       <c r="G44" s="3">
-        <v>17693.456552400003</v>
+        <v>27680.236950999999</v>
       </c>
       <c r="H44" s="3">
-        <v>27680.236950999999</v>
+        <v>338.953844</v>
       </c>
       <c r="I44" s="3">
-        <v>338.953844</v>
+        <v>1900</v>
       </c>
       <c r="J44" s="3">
-        <v>1900</v>
-      </c>
-      <c r="K44" s="3">
         <v>10986.253129000001</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>51</v>
       </c>
+      <c r="B45" s="3">
+        <v>92982.445000000007</v>
+      </c>
       <c r="C45" s="3">
-        <v>92982.445000000007</v>
+        <v>0</v>
       </c>
       <c r="D45" s="3">
-        <v>0</v>
-      </c>
-      <c r="E45" s="3">
         <v>1999.99553367</v>
       </c>
-      <c r="F45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3">
+        <v>494.63875000000002</v>
+      </c>
       <c r="G45" s="3">
-        <v>494.63875000000002</v>
+        <v>3581.9168079999999</v>
       </c>
       <c r="H45" s="3">
-        <v>3581.9168079999999</v>
+        <v>300.981424</v>
       </c>
       <c r="I45" s="3">
-        <v>300.981424</v>
+        <v>1900</v>
       </c>
       <c r="J45" s="3">
-        <v>1900</v>
-      </c>
-      <c r="K45" s="3">
         <v>10986.253129000001</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>52</v>
       </c>
+      <c r="B46" s="3">
+        <v>5496.732</v>
+      </c>
       <c r="C46" s="3">
-        <v>5496.732</v>
+        <v>0</v>
       </c>
       <c r="D46" s="3">
-        <v>0</v>
-      </c>
-      <c r="E46" s="3">
         <v>749.99799091</v>
       </c>
-      <c r="F46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3">
+        <v>0</v>
+      </c>
       <c r="G46" s="3">
-        <v>0</v>
+        <v>3376.7100230000001</v>
       </c>
       <c r="H46" s="3">
-        <v>3376.7100230000001</v>
+        <v>37.97242</v>
       </c>
       <c r="I46" s="3">
-        <v>37.97242</v>
+        <v>0</v>
       </c>
       <c r="J46" s="3">
         <v>0</v>
       </c>
-      <c r="K46" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>53</v>
       </c>
+      <c r="B47" s="3">
+        <v>17908.334515439998</v>
+      </c>
       <c r="C47" s="3">
-        <v>17908.334515439998</v>
+        <v>25615.927377960001</v>
       </c>
       <c r="D47" s="3">
-        <v>25615.927377960001</v>
-      </c>
-      <c r="E47" s="3">
-        <v>0</v>
-      </c>
-      <c r="F47" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3">
+        <v>17198.817802400001</v>
+      </c>
       <c r="G47" s="3">
-        <v>17198.817802400001</v>
+        <v>20721.610120000001</v>
       </c>
       <c r="H47" s="3">
-        <v>20721.610120000001</v>
+        <v>0</v>
       </c>
       <c r="I47" s="3">
         <v>0</v>
@@ -2335,24 +2338,24 @@
       <c r="J47" s="3">
         <v>0</v>
       </c>
-      <c r="K47" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="B48" s="3">
+        <v>0</v>
+      </c>
       <c r="C48" s="3">
         <v>0</v>
       </c>
       <c r="D48" s="3">
         <v>0</v>
       </c>
-      <c r="E48" s="3">
-        <v>0</v>
-      </c>
-      <c r="F48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3">
+        <v>0</v>
+      </c>
       <c r="G48" s="3">
         <v>0</v>
       </c>
@@ -2365,144 +2368,144 @@
       <c r="J48" s="3">
         <v>0</v>
       </c>
-      <c r="K48" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>55</v>
       </c>
+      <c r="B49" s="3">
+        <v>1319058.3509434299</v>
+      </c>
       <c r="C49" s="3">
-        <v>1319058.3509434299</v>
+        <v>470699.91261696001</v>
       </c>
       <c r="D49" s="3">
-        <v>470699.91261696001</v>
-      </c>
-      <c r="E49" s="3">
         <v>837540.99521601002</v>
       </c>
-      <c r="F49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3">
+        <v>496307.77671740996</v>
+      </c>
       <c r="G49" s="3">
-        <v>496307.77671740996</v>
+        <v>657929.59389581007</v>
       </c>
       <c r="H49" s="3">
-        <v>657929.59389581007</v>
+        <v>441999.99297999998</v>
       </c>
       <c r="I49" s="3">
-        <v>441999.99297999998</v>
+        <v>773701.07219154004</v>
       </c>
       <c r="J49" s="3">
-        <v>773701.07219154004</v>
-      </c>
-      <c r="K49" s="3">
         <v>938526.50535306998</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>56</v>
       </c>
+      <c r="B50" s="3">
+        <v>390887.86101416999</v>
+      </c>
       <c r="C50" s="3">
-        <v>390887.86101416999</v>
+        <v>53590.211092160003</v>
       </c>
       <c r="D50" s="3">
-        <v>53590.211092160003</v>
-      </c>
-      <c r="E50" s="3">
         <v>45667.569381510002</v>
       </c>
-      <c r="F50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3">
+        <v>63194.541382440002</v>
+      </c>
       <c r="G50" s="3">
-        <v>63194.541382440002</v>
+        <v>56138.257067370003</v>
       </c>
       <c r="H50" s="3">
-        <v>56138.257067370003</v>
+        <v>54405.355025540004</v>
       </c>
       <c r="I50" s="3">
-        <v>54405.355025540004</v>
+        <v>39356.820507789998</v>
       </c>
       <c r="J50" s="3">
-        <v>39356.820507789998</v>
-      </c>
-      <c r="K50" s="3">
         <v>190928.50766067</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>57</v>
       </c>
+      <c r="B51" s="3">
+        <v>524737.40642630996</v>
+      </c>
       <c r="C51" s="3">
-        <v>524737.40642630996</v>
+        <v>54390.211092160003</v>
       </c>
       <c r="D51" s="3">
-        <v>54390.211092160003</v>
-      </c>
-      <c r="E51" s="3">
         <v>48489.313187510001</v>
       </c>
-      <c r="F51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3">
+        <v>68786.891382440008</v>
+      </c>
       <c r="G51" s="3">
-        <v>68786.891382440008</v>
+        <v>65559.673584820004</v>
       </c>
       <c r="H51" s="3">
-        <v>65559.673584820004</v>
+        <v>56130.355025540004</v>
       </c>
       <c r="I51" s="3">
-        <v>56130.355025540004</v>
+        <v>45934.855801969999</v>
       </c>
       <c r="J51" s="3">
-        <v>45934.855801969999</v>
-      </c>
-      <c r="K51" s="3">
         <v>191928.50766067</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>58</v>
       </c>
+      <c r="B52" s="3">
+        <v>524737.40642630996</v>
+      </c>
       <c r="C52" s="3">
-        <v>524737.40642630996</v>
+        <v>47582.803059689999</v>
       </c>
       <c r="D52" s="3">
-        <v>47582.803059689999</v>
-      </c>
-      <c r="E52" s="3">
         <v>48489.313187510001</v>
       </c>
-      <c r="F52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3">
+        <v>64286.891382440001</v>
+      </c>
       <c r="G52" s="3">
-        <v>64286.891382440001</v>
+        <v>65559.673584820004</v>
       </c>
       <c r="H52" s="3">
-        <v>65559.673584820004</v>
+        <v>55680.355025540004</v>
       </c>
       <c r="I52" s="3">
-        <v>55680.355025540004</v>
+        <v>45934.855801969999</v>
       </c>
       <c r="J52" s="3">
-        <v>45934.855801969999</v>
-      </c>
-      <c r="K52" s="3">
         <v>191928.50766067</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>59</v>
       </c>
+      <c r="B53" s="3">
+        <v>0</v>
+      </c>
       <c r="C53" s="3">
         <v>0</v>
       </c>
       <c r="D53" s="3">
         <v>0</v>
       </c>
-      <c r="E53" s="3">
-        <v>0</v>
-      </c>
-      <c r="F53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3">
+        <v>0</v>
+      </c>
       <c r="G53" s="3">
         <v>0</v>
       </c>
@@ -2515,24 +2518,24 @@
       <c r="J53" s="3">
         <v>0</v>
       </c>
-      <c r="K53" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>60</v>
       </c>
+      <c r="B54" s="3">
+        <v>0</v>
+      </c>
       <c r="C54" s="3">
         <v>0</v>
       </c>
       <c r="D54" s="3">
         <v>0</v>
       </c>
-      <c r="E54" s="3">
-        <v>0</v>
-      </c>
-      <c r="F54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3">
+        <v>0</v>
+      </c>
       <c r="G54" s="3">
         <v>0</v>
       </c>
@@ -2545,26 +2548,26 @@
       <c r="J54" s="3">
         <v>0</v>
       </c>
-      <c r="K54" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>61</v>
       </c>
+      <c r="B55" s="3">
+        <v>0</v>
+      </c>
       <c r="C55" s="3">
         <v>0</v>
       </c>
       <c r="D55" s="3">
         <v>0</v>
       </c>
-      <c r="E55" s="3">
-        <v>0</v>
-      </c>
-      <c r="F55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3">
+        <v>4500</v>
+      </c>
       <c r="G55" s="3">
-        <v>4500</v>
+        <v>0</v>
       </c>
       <c r="H55" s="3">
         <v>0</v>
@@ -2575,84 +2578,84 @@
       <c r="J55" s="3">
         <v>0</v>
       </c>
-      <c r="K55" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>62</v>
       </c>
+      <c r="B56" s="3">
+        <v>0</v>
+      </c>
       <c r="C56" s="3">
-        <v>0</v>
+        <v>6807.4080324699999</v>
       </c>
       <c r="D56" s="3">
-        <v>6807.4080324699999</v>
-      </c>
-      <c r="E56" s="3">
-        <v>0</v>
-      </c>
-      <c r="F56" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3">
+        <v>0</v>
+      </c>
       <c r="G56" s="3">
         <v>0</v>
       </c>
       <c r="H56" s="3">
-        <v>0</v>
+        <v>450</v>
       </c>
       <c r="I56" s="3">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="J56" s="3">
         <v>0</v>
       </c>
-      <c r="K56" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>63</v>
       </c>
+      <c r="B57" s="3">
+        <v>133849.54541214</v>
+      </c>
       <c r="C57" s="3">
-        <v>133849.54541214</v>
+        <v>800</v>
       </c>
       <c r="D57" s="3">
-        <v>800</v>
-      </c>
-      <c r="E57" s="3">
         <v>2821.7438059999999</v>
       </c>
-      <c r="F57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3">
+        <v>5592.35</v>
+      </c>
       <c r="G57" s="3">
-        <v>5592.35</v>
+        <v>9421.4165174500013</v>
       </c>
       <c r="H57" s="3">
-        <v>9421.4165174500013</v>
+        <v>1725</v>
       </c>
       <c r="I57" s="3">
-        <v>1725</v>
+        <v>6578.0352941800002</v>
       </c>
       <c r="J57" s="3">
-        <v>6578.0352941800002</v>
-      </c>
-      <c r="K57" s="3">
         <v>1000</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>64</v>
       </c>
+      <c r="B58" s="3">
+        <v>0</v>
+      </c>
       <c r="C58" s="3">
         <v>0</v>
       </c>
       <c r="D58" s="3">
         <v>0</v>
       </c>
-      <c r="E58" s="3">
-        <v>0</v>
-      </c>
-      <c r="F58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3">
+        <v>0</v>
+      </c>
       <c r="G58" s="3">
         <v>0</v>
       </c>
@@ -2665,54 +2668,54 @@
       <c r="J58" s="3">
         <v>0</v>
       </c>
-      <c r="K58" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>65</v>
       </c>
+      <c r="B59" s="3">
+        <v>8849.5454121399998</v>
+      </c>
       <c r="C59" s="3">
-        <v>8849.5454121399998</v>
+        <v>800</v>
       </c>
       <c r="D59" s="3">
-        <v>800</v>
-      </c>
-      <c r="E59" s="3">
         <v>2500</v>
       </c>
-      <c r="F59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3">
+        <v>0</v>
+      </c>
       <c r="G59" s="3">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="H59" s="3">
-        <v>175</v>
+        <v>1725</v>
       </c>
       <c r="I59" s="3">
-        <v>1725</v>
+        <v>0</v>
       </c>
       <c r="J59" s="3">
-        <v>0</v>
-      </c>
-      <c r="K59" s="3">
         <v>1000</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>66</v>
       </c>
+      <c r="B60" s="3">
+        <v>125000</v>
+      </c>
       <c r="C60" s="3">
-        <v>125000</v>
+        <v>0</v>
       </c>
       <c r="D60" s="3">
-        <v>0</v>
-      </c>
-      <c r="E60" s="3">
         <v>321.74380600000001</v>
       </c>
-      <c r="F60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3">
+        <v>0</v>
+      </c>
       <c r="G60" s="3">
         <v>0</v>
       </c>
@@ -2720,29 +2723,29 @@
         <v>0</v>
       </c>
       <c r="I60" s="3">
-        <v>0</v>
+        <v>6578.0352941800002</v>
       </c>
       <c r="J60" s="3">
-        <v>6578.0352941800002</v>
-      </c>
-      <c r="K60" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>67</v>
       </c>
+      <c r="B61" s="3">
+        <v>0</v>
+      </c>
       <c r="C61" s="3">
         <v>0</v>
       </c>
       <c r="D61" s="3">
         <v>0</v>
       </c>
-      <c r="E61" s="3">
-        <v>0</v>
-      </c>
-      <c r="F61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3">
+        <v>0</v>
+      </c>
       <c r="G61" s="3">
         <v>0</v>
       </c>
@@ -2755,24 +2758,24 @@
       <c r="J61" s="3">
         <v>0</v>
       </c>
-      <c r="K61" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>67</v>
       </c>
+      <c r="B62" s="3">
+        <v>0</v>
+      </c>
       <c r="C62" s="3">
         <v>0</v>
       </c>
       <c r="D62" s="3">
         <v>0</v>
       </c>
-      <c r="E62" s="3">
-        <v>0</v>
-      </c>
-      <c r="F62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3">
+        <v>0</v>
+      </c>
       <c r="G62" s="3">
         <v>0</v>
       </c>
@@ -2785,26 +2788,26 @@
       <c r="J62" s="3">
         <v>0</v>
       </c>
-      <c r="K62" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>68</v>
       </c>
+      <c r="B63" s="3">
+        <v>0</v>
+      </c>
       <c r="C63" s="3">
         <v>0</v>
       </c>
       <c r="D63" s="3">
         <v>0</v>
       </c>
-      <c r="E63" s="3">
-        <v>0</v>
-      </c>
-      <c r="F63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3">
+        <v>5592.35</v>
+      </c>
       <c r="G63" s="3">
-        <v>5592.35</v>
+        <v>0</v>
       </c>
       <c r="H63" s="3">
         <v>0</v>
@@ -2813,9 +2816,6 @@
         <v>0</v>
       </c>
       <c r="J63" s="3">
-        <v>0</v>
-      </c>
-      <c r="K63" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>